<commit_message>
recreating statistics, also available now through sparql
</commit_message>
<xml_diff>
--- a/evaluation/results.xlsx
+++ b/evaluation/results.xlsx
@@ -56,7 +56,7 @@
     <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -81,6 +81,11 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -218,6 +223,17 @@
   <c:roundedCorners val="0"/>
   <c:chart>
     <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.131101333699986"/>
+          <c:y val="0.0419906687402799"/>
+          <c:w val="0.848755671662313"/>
+          <c:h val="0.810708731393024"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -663,16 +679,62 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="74464646"/>
-        <c:axId val="91470968"/>
+        <c:axId val="24723055"/>
+        <c:axId val="52885567"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="74464646"/>
+        <c:axId val="24723055"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Number of deployed services</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.386196466625421"/>
+              <c:y val="0.906364545151616"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -702,14 +764,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91470968"/>
+        <c:crossAx val="52885567"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91470968"/>
+        <c:axId val="52885567"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -724,6 +786,52 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Deploament time in seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.0208977796109163"/>
+              <c:y val="0.679440186604465"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -753,7 +861,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74464646"/>
+        <c:crossAx val="24723055"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -791,9 +899,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>326160</xdr:colOff>
+      <xdr:colOff>325800</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>68400</xdr:rowOff>
+      <xdr:rowOff>68040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -801,8 +909,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4337640" y="1866600"/>
-        <a:ext cx="5513400" cy="3241080"/>
+        <a:off x="4271040" y="1866600"/>
+        <a:ext cx="5236560" cy="3240720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -823,19 +931,21 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L7" activeCellId="0" sqref="L7"/>
+      <selection pane="topLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.32142857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.18367346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>